<commit_message>
Ernest's part is done :)
</commit_message>
<xml_diff>
--- a/Projekt1-Wtykło-Dąbrowski-2.xlsx
+++ b/Projekt1-Wtykło-Dąbrowski-2.xlsx
@@ -475,16 +475,16 @@
     <t>Cost Hata - metropolitan (UPLINK)</t>
   </si>
   <si>
-    <t>Dopuszczalne tłumienie trasy 75% miejsc - PODMIEJSKI</t>
+    <t>Dopuszczalne tłumienie trasy  50% miejsc - Suburban</t>
   </si>
   <si>
-    <t>Dopuszczalne tłumienie trasy  50% miejsc - PODMIEJSKI</t>
+    <t>Dopuszczalne tłumienie trasy 75% miejsc - Suburban</t>
   </si>
   <si>
-    <t>Dopuszczalne tłumienie trasy  50% miejsc - METROPOLIA</t>
+    <t>Dopuszczalne tłumienie trasy  50% miejsc - Metropolitan</t>
   </si>
   <si>
-    <t>Dopuszczalne tłumienie trasy 75% miejsc - METROPOLIA</t>
+    <t>Dopuszczalne tłumienie trasy 75% miejsc - Metropolitan</t>
   </si>
 </sst>
 </file>
@@ -3983,8 +3983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH772"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8592,7 +8592,7 @@
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A68" s="286" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B68" s="216">
         <v>147.62</v>
@@ -8667,7 +8667,7 @@
     </row>
     <row r="69" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="287" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B69" s="218">
         <v>142.62</v>

</xml_diff>